<commit_message>
26 de marzo 2022
</commit_message>
<xml_diff>
--- a/Tercer Bimestre/Testing l/Template casos de prueba y defectos.xlsx
+++ b/Tercer Bimestre/Testing l/Template casos de prueba y defectos.xlsx
@@ -238,15 +238,18 @@
       <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <color theme="1"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <color theme="1"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
     <font/>
     <font>
@@ -408,7 +411,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="29">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -471,12 +474,6 @@
     <xf borderId="11" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="12" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="13" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
     <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
@@ -757,15 +754,15 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="18.29"/>
-    <col customWidth="1" min="2" max="2" width="18.0"/>
-    <col customWidth="1" min="3" max="3" width="20.14"/>
-    <col customWidth="1" min="4" max="4" width="23.57"/>
-    <col customWidth="1" min="5" max="5" width="22.29"/>
-    <col customWidth="1" min="6" max="6" width="22.57"/>
-    <col customWidth="1" min="7" max="7" width="18.29"/>
+    <col customWidth="1" min="1" max="1" width="16.0"/>
+    <col customWidth="1" min="2" max="2" width="15.75"/>
+    <col customWidth="1" min="3" max="3" width="17.63"/>
+    <col customWidth="1" min="4" max="4" width="20.63"/>
+    <col customWidth="1" min="5" max="5" width="19.5"/>
+    <col customWidth="1" min="6" max="6" width="19.75"/>
+    <col customWidth="1" min="7" max="7" width="16.0"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1012,14 +1009,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="29.86"/>
-    <col customWidth="1" min="3" max="3" width="40.14"/>
-    <col customWidth="1" min="4" max="4" width="23.71"/>
-    <col customWidth="1" min="6" max="6" width="49.29"/>
-    <col customWidth="1" min="7" max="7" width="51.57"/>
-    <col customWidth="1" min="8" max="8" width="21.71"/>
+    <col customWidth="1" min="2" max="2" width="26.13"/>
+    <col customWidth="1" min="3" max="3" width="35.13"/>
+    <col customWidth="1" min="4" max="4" width="20.75"/>
+    <col customWidth="1" min="6" max="6" width="43.13"/>
+    <col customWidth="1" min="7" max="7" width="45.13"/>
+    <col customWidth="1" min="8" max="8" width="19.0"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -1154,9 +1151,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="4" max="4" width="18.71"/>
+    <col customWidth="1" min="4" max="4" width="16.38"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1258,14 +1255,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="28.71"/>
-    <col customWidth="1" min="3" max="3" width="46.86"/>
-    <col customWidth="1" min="4" max="4" width="20.86"/>
-    <col customWidth="1" min="5" max="5" width="20.57"/>
-    <col customWidth="1" min="8" max="8" width="21.0"/>
-    <col customWidth="1" min="11" max="12" width="15.71"/>
+    <col customWidth="1" min="2" max="2" width="25.13"/>
+    <col customWidth="1" min="3" max="3" width="41.0"/>
+    <col customWidth="1" min="4" max="4" width="18.25"/>
+    <col customWidth="1" min="5" max="5" width="18.0"/>
+    <col customWidth="1" min="8" max="8" width="18.38"/>
+    <col customWidth="1" min="11" max="12" width="13.75"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -1341,41 +1338,41 @@
       <c r="R3" s="9"/>
     </row>
     <row r="4">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="30" t="s">
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="28" t="s">
         <v>56</v>
       </c>
       <c r="G4" s="7"/>
       <c r="H4" s="8"/>
-      <c r="I4" s="28" t="s">
+      <c r="I4" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="J4" s="28" t="s">
+      <c r="J4" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="K4" s="28" t="s">
+      <c r="K4" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="L4" s="28" t="s">
+      <c r="L4" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="M4" s="28" t="s">
+      <c r="M4" s="2" t="s">
         <v>60</v>
       </c>
       <c r="N4" s="4"/>
       <c r="O4" s="4"/>
-      <c r="P4" s="28" t="s">
+      <c r="P4" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="Q4" s="28" t="s">
+      <c r="Q4" s="2" t="s">
         <v>62</v>
       </c>
       <c r="R4" s="4"/>
@@ -1391,14 +1388,14 @@
     <mergeCell ref="I2:I3"/>
     <mergeCell ref="F4:H4"/>
     <mergeCell ref="Q2:Q3"/>
-    <mergeCell ref="P2:P3"/>
+    <mergeCell ref="R2:R3"/>
     <mergeCell ref="J2:J3"/>
     <mergeCell ref="K2:K3"/>
     <mergeCell ref="L2:L3"/>
     <mergeCell ref="M2:M3"/>
     <mergeCell ref="N2:N3"/>
     <mergeCell ref="O2:O3"/>
-    <mergeCell ref="R2:R3"/>
+    <mergeCell ref="P2:P3"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>